<commit_message>
Reading feature file from Excel/ read and write text files/ add data to excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/datafiles/ExcelB.xlsx
+++ b/src/test/resources/datafiles/ExcelB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t>first_name</t>
   </si>
@@ -318,6 +318,24 @@
   </si>
   <si>
     <t>849-87-0649</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>World!!!</t>
+  </si>
+  <si>
+    <t>ahmet</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>ozyurek</t>
   </si>
 </sst>
 </file>
@@ -362,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -788,6 +806,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>